<commit_message>
Alterei o nome de algumas variaveis
</commit_message>
<xml_diff>
--- a/Test-Case-Template.xlsx
+++ b/Test-Case-Template.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/201901829_estudantes_ips_pt/Documents/Desktop/Aulas/1ºAno/1º Semestre/AFP/Projeto_Final/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B6E8F44EC446E0BBFAC07D36D4E0E0E653884751" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="TestCaseTemplate" sheetId="1" r:id="rId4"/>
+    <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -87,29 +96,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="16.0"/>
+      <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Verdana"/>
     </font>
@@ -119,7 +131,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -135,27 +147,39 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -165,6 +189,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -179,49 +204,47 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -411,114 +434,116 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.86"/>
-    <col customWidth="1" min="2" max="2" width="19.14"/>
-    <col customWidth="1" min="3" max="3" width="7.43"/>
-    <col customWidth="1" min="4" max="4" width="26.57"/>
-    <col customWidth="1" min="5" max="5" width="13.71"/>
-    <col customWidth="1" min="6" max="6" width="34.57"/>
-    <col customWidth="1" min="7" max="8" width="15.29"/>
-    <col customWidth="1" min="9" max="9" width="17.14"/>
-    <col customWidth="1" min="10" max="10" width="9.29"/>
-    <col customWidth="1" min="11" max="11" width="16.0"/>
-    <col customWidth="1" min="12" max="27" width="8.71"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" customWidth="1"/>
+    <col min="7" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" ht="14.4">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="90.0" customHeight="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:11" ht="90" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1506,9 +1531,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>